<commit_message>
missing DFTs added except m06l
</commit_message>
<xml_diff>
--- a/XLSX/data.xlsx
+++ b/XLSX/data.xlsx
@@ -1113,13 +1113,13 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>91.62728000001152</v>
+        <v>91.76511000001142</v>
       </c>
       <c r="F25" t="n">
-        <v>544.8580400000083</v>
+        <v>545.136250000013</v>
       </c>
       <c r="G25" t="n">
-        <v>1037.648820000015</v>
+        <v>1037.833360000008</v>
       </c>
     </row>
     <row r="26">
@@ -1572,13 +1572,13 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>87.12549999999996</v>
+        <v>0.7995599999999214</v>
       </c>
       <c r="F42" t="n">
-        <v>507.5817799999998</v>
+        <v>357.6212700000001</v>
       </c>
       <c r="G42" t="n">
-        <v>1113.32031</v>
+        <v>1066.034549999999</v>
       </c>
     </row>
     <row r="43">
@@ -2220,13 +2220,13 @@
         <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>851.7495400000143</v>
+        <v>852.3717399999953</v>
       </c>
       <c r="F66" t="n">
-        <v>1054.837910000003</v>
+        <v>1055.130289999994</v>
       </c>
       <c r="G66" t="n">
-        <v>1381.011330000007</v>
+        <v>1381.318850000014</v>
       </c>
     </row>
     <row r="67">
@@ -2679,13 +2679,13 @@
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>861.3107499999994</v>
+        <v>875.3741300000008</v>
       </c>
       <c r="F83" t="n">
-        <v>1278.94618</v>
+        <v>1484.8131</v>
       </c>
       <c r="G83" t="n">
-        <v>1296.90503</v>
+        <v>1437.637390000001</v>
       </c>
     </row>
     <row r="84">
@@ -3327,13 +3327,13 @@
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>-88.73047999998107</v>
+        <v>-88.32606000004262</v>
       </c>
       <c r="F107" t="n">
-        <v>205.9470000000374</v>
+        <v>206.5440700000067</v>
       </c>
       <c r="G107" t="n">
-        <v>-3.113799999994171</v>
+        <v>-3.223649999995359</v>
       </c>
     </row>
     <row r="108">
@@ -3786,13 +3786,13 @@
         <v>0</v>
       </c>
       <c r="E124" t="n">
-        <v>113.2039299999974</v>
+        <v>485.4063500000017</v>
       </c>
       <c r="F124" t="n">
-        <v>241.6077100000003</v>
+        <v>429.9156400000008</v>
       </c>
       <c r="G124" t="n">
-        <v>202.6991699999989</v>
+        <v>607.8611800000004</v>
       </c>
     </row>
     <row r="125">
@@ -4434,13 +4434,13 @@
         <v>0</v>
       </c>
       <c r="E148" t="n">
-        <v>277.6282199999969</v>
+        <v>277.3747899999961</v>
       </c>
       <c r="F148" t="n">
-        <v>740.7580699999983</v>
+        <v>741.115839999999</v>
       </c>
       <c r="G148" t="n">
-        <v>866.4250200000013</v>
+        <v>866.887779999999</v>
       </c>
     </row>
     <row r="149">
@@ -4893,13 +4893,13 @@
         <v>0</v>
       </c>
       <c r="E165" t="n">
-        <v>260.3266999999993</v>
+        <v>170.5642100000002</v>
       </c>
       <c r="F165" t="n">
-        <v>744.7893799999994</v>
+        <v>565.6927200000003</v>
       </c>
       <c r="G165" t="n">
-        <v>890.5539199999995</v>
+        <v>850.29909</v>
       </c>
     </row>
     <row r="166">
@@ -5541,13 +5541,13 @@
         <v>0</v>
       </c>
       <c r="E189" t="n">
-        <v>119.5182199999891</v>
+        <v>118.7176699999952</v>
       </c>
       <c r="F189" t="n">
-        <v>275.6365999999986</v>
+        <v>275.0136699999928</v>
       </c>
       <c r="G189" t="n">
-        <v>1151.97809</v>
+        <v>1151.066180000001</v>
       </c>
     </row>
     <row r="190">
@@ -6000,13 +6000,13 @@
         <v>0</v>
       </c>
       <c r="E206" t="n">
-        <v>127.5752099999998</v>
+        <v>210.1019500000003</v>
       </c>
       <c r="F206" t="n">
-        <v>523.0785199999985</v>
+        <v>739.9147500000005</v>
       </c>
       <c r="G206" t="n">
-        <v>1157.804909999999</v>
+        <v>1193.81924</v>
       </c>
     </row>
     <row r="207">
@@ -6648,13 +6648,13 @@
         <v>0</v>
       </c>
       <c r="E230" t="n">
-        <v>-1319.332129999992</v>
+        <v>-1320.545800000005</v>
       </c>
       <c r="F230" t="n">
-        <v>-204.9294099999912</v>
+        <v>-204.9000399999983</v>
       </c>
       <c r="G230" t="n">
-        <v>-1510.387919999999</v>
+        <v>-1509.300210000006</v>
       </c>
     </row>
     <row r="231">
@@ -7107,13 +7107,13 @@
         <v>0</v>
       </c>
       <c r="E247" t="n">
-        <v>-986.9600100000007</v>
+        <v>-536.41863</v>
       </c>
       <c r="F247" t="n">
-        <v>-145.4788300000001</v>
+        <v>26.81366000000018</v>
       </c>
       <c r="G247" t="n">
-        <v>-1173.73392</v>
+        <v>-672.0787399999999</v>
       </c>
     </row>
     <row r="248">
@@ -7755,13 +7755,13 @@
         <v>0</v>
       </c>
       <c r="E271" t="n">
-        <v>550.3979100000009</v>
+        <v>491.7549799999996</v>
       </c>
       <c r="F271" t="n">
-        <v>1235.1141</v>
+        <v>1194.501589999998</v>
       </c>
       <c r="G271" t="n">
-        <v>1000.198610000002</v>
+        <v>1064.741739999999</v>
       </c>
     </row>
     <row r="272">
@@ -8214,13 +8214,13 @@
         <v>0</v>
       </c>
       <c r="E288" t="n">
-        <v>417.6165700000008</v>
+        <v>289.3396299999997</v>
       </c>
       <c r="F288" t="n">
-        <v>1311.47678</v>
+        <v>906.1302499999995</v>
       </c>
       <c r="G288" t="n">
-        <v>1032.630090000001</v>
+        <v>1093.32229</v>
       </c>
     </row>
     <row r="289">
@@ -8862,13 +8862,13 @@
         <v>0</v>
       </c>
       <c r="E312" t="n">
-        <v>129.855340000006</v>
+        <v>221.5700100000007</v>
       </c>
       <c r="F312" t="n">
-        <v>-49.53694999999669</v>
+        <v>2.335670000000789</v>
       </c>
       <c r="G312" t="n">
-        <v>1163.953390000003</v>
+        <v>1282.661750000002</v>
       </c>
     </row>
     <row r="313">
@@ -9321,13 +9321,13 @@
         <v>0</v>
       </c>
       <c r="E329" t="n">
-        <v>70.63134999999932</v>
+        <v>185.6881799999996</v>
       </c>
       <c r="F329" t="n">
-        <v>164.5939300000006</v>
+        <v>554.6742800000004</v>
       </c>
       <c r="G329" t="n">
-        <v>1149.77775</v>
+        <v>1274.98194</v>
       </c>
     </row>
     <row r="330">
@@ -9969,13 +9969,13 @@
         <v>0</v>
       </c>
       <c r="E353" t="n">
-        <v>-1794.357780000013</v>
+        <v>-1803.087160000004</v>
       </c>
       <c r="F353" t="n">
-        <v>-285.594830000008</v>
+        <v>-262.9798600000015</v>
       </c>
       <c r="G353" t="n">
-        <v>-1968.86241</v>
+        <v>-2109.081889999999</v>
       </c>
     </row>
     <row r="354">
@@ -10428,13 +10428,13 @@
         <v>0</v>
       </c>
       <c r="E370" t="n">
-        <v>-1557.401509999998</v>
+        <v>-907.2236999999994</v>
       </c>
       <c r="F370" t="n">
-        <v>-277.4206600000007</v>
+        <v>-74.98568000000105</v>
       </c>
       <c r="G370" t="n">
-        <v>-1768.07269</v>
+        <v>-1051.706280000001</v>
       </c>
     </row>
   </sheetData>
@@ -11315,13 +11315,13 @@
         <v>-1422.551769999874</v>
       </c>
       <c r="D24" t="n">
-        <v>1761045.76682</v>
+        <v>-248.0637099998959</v>
       </c>
       <c r="E24" t="n">
         <v>-760.5803200000216</v>
       </c>
       <c r="F24" t="n">
-        <v>1761045.92983</v>
+        <v>-323.2353499999547</v>
       </c>
       <c r="G24" t="n">
         <v>-253.2016199999556</v>
@@ -11333,7 +11333,7 @@
         <v>-481.2750999998689</v>
       </c>
       <c r="J24" t="n">
-        <v>6669670.321529999</v>
+        <v>-432.968229999938</v>
       </c>
     </row>
     <row r="25">
@@ -11348,28 +11348,28 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-1656158.92733</v>
+        <v>-2008.259559999971</v>
       </c>
       <c r="D25" t="n">
-        <v>-1633338.06888</v>
+        <v>-782.5278700000808</v>
       </c>
       <c r="E25" t="n">
-        <v>79524.36195999999</v>
+        <v>-1689.518819999975</v>
       </c>
       <c r="F25" t="n">
-        <v>-1655856.28511</v>
+        <v>1037.194200000044</v>
       </c>
       <c r="G25" t="n">
-        <v>-1657006.39814</v>
+        <v>-1452.163440000078</v>
       </c>
       <c r="H25" t="n">
-        <v>-1657487.77256</v>
+        <v>-1788.926649999937</v>
       </c>
       <c r="I25" t="n">
-        <v>-1657623.35973</v>
+        <v>-1979.904039999965</v>
       </c>
       <c r="J25" t="n">
-        <v>79519.99673</v>
+        <v>-1888.00386999992</v>
       </c>
     </row>
     <row r="26">
@@ -11960,28 +11960,28 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>-1988.321949999944</v>
+        <v>-1602.283920000039</v>
       </c>
       <c r="D42" t="n">
-        <v>-733.7068399998943</v>
+        <v>-461.8997799999898</v>
       </c>
       <c r="E42" t="n">
-        <v>-1316.109339999963</v>
+        <v>-944.7564099999192</v>
       </c>
       <c r="F42" t="n">
-        <v>-1084.895479999891</v>
+        <v>-680.2574699999493</v>
       </c>
       <c r="G42" t="n">
-        <v>-1012.085199999864</v>
+        <v>-599.2692000000734</v>
       </c>
       <c r="H42" t="n">
-        <v>-1536.316810000012</v>
+        <v>-990.8328300000315</v>
       </c>
       <c r="I42" t="n">
-        <v>-1295.758189999793</v>
+        <v>-773.1748300000203</v>
       </c>
       <c r="J42" t="n">
-        <v>-1237.938529999895</v>
+        <v>-753.153470000095</v>
       </c>
     </row>
     <row r="43">
@@ -12968,16 +12968,16 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1776728.33309</v>
+        <v>-677.2798500000547</v>
       </c>
       <c r="D70" t="n">
-        <v>1776728.04383</v>
+        <v>-127.2843700000053</v>
       </c>
       <c r="E70" t="n">
         <v>-377.0115000000267</v>
       </c>
       <c r="F70" t="n">
-        <v>1776727.61977</v>
+        <v>-130.5510400000216</v>
       </c>
       <c r="G70" t="n">
         <v>-109.0224400000288</v>
@@ -13004,28 +13004,28 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>-1359.56172000002</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>-344.3006599999059</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>-643.3105200000319</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>-571.3335800000685</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>-1683.283910000004</v>
       </c>
       <c r="H71" t="n">
-        <v>-1686268.58851</v>
+        <v>-1306.376230000076</v>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>-1744.298270000062</v>
       </c>
       <c r="J71" t="n">
-        <v>29976.30221</v>
+        <v>229.1676999999765</v>
       </c>
     </row>
     <row r="72">
@@ -13616,28 +13616,28 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>-1188.983459999833</v>
+        <v>-918.746980000054</v>
       </c>
       <c r="D88" t="n">
-        <v>-557.2839099999558</v>
+        <v>-368.5052500000139</v>
       </c>
       <c r="E88" t="n">
-        <v>-876.3169399998465</v>
+        <v>-617.6957499999194</v>
       </c>
       <c r="F88" t="n">
-        <v>-770.0625499997913</v>
+        <v>-471.9400299999292</v>
       </c>
       <c r="G88" t="n">
-        <v>-761.9169599998603</v>
+        <v>-449.9057599999667</v>
       </c>
       <c r="H88" t="n">
-        <v>-1197.112269999918</v>
+        <v>-779.8869400000422</v>
       </c>
       <c r="I88" t="n">
-        <v>-921.1868699999615</v>
+        <v>-537.0862099999476</v>
       </c>
       <c r="J88" t="n">
-        <v>-1035.042169999902</v>
+        <v>-641.7727200000862</v>
       </c>
     </row>
     <row r="89">
@@ -13976,7 +13976,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>-4365.563960000145</v>
+        <v>-1617.095710000145</v>
       </c>
       <c r="D98" t="n">
         <v>-460.2194400001207</v>
@@ -14627,16 +14627,16 @@
         <v>-1256.935179999989</v>
       </c>
       <c r="D116" t="n">
-        <v>1776212.44722</v>
+        <v>-115.6393300000538</v>
       </c>
       <c r="E116" t="n">
         <v>-557.5083800000335</v>
       </c>
       <c r="F116" t="n">
-        <v>1230313.77521</v>
+        <v>-159.0454699999775</v>
       </c>
       <c r="G116" t="n">
-        <v>1776211.65043</v>
+        <v>-141.5534199999726</v>
       </c>
       <c r="H116" t="n">
         <v>-744.2008800000579</v>
@@ -14645,7 +14645,7 @@
         <v>-287.5479999999833</v>
       </c>
       <c r="J116" t="n">
-        <v>-18438.02645000005</v>
+        <v>-448.5602200000507</v>
       </c>
     </row>
     <row r="117">
@@ -14660,28 +14660,28 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>-1658168.10297</v>
+        <v>-2715.192510000056</v>
       </c>
       <c r="D117" t="n">
-        <v>-222046.76032</v>
+        <v>1553.528099999957</v>
       </c>
       <c r="E117" t="n">
-        <v>-1658020.173</v>
+        <v>-1812.590479999883</v>
       </c>
       <c r="F117" t="n">
-        <v>14347.64821</v>
+        <v>-293.89284000003</v>
       </c>
       <c r="G117" t="n">
-        <v>14414.70007</v>
+        <v>2959.436419999975</v>
       </c>
       <c r="H117" t="n">
-        <v>14201.91924</v>
+        <v>-1814.720170000019</v>
       </c>
       <c r="I117" t="n">
-        <v>13877.65077</v>
+        <v>180.6979499999937</v>
       </c>
       <c r="J117" t="n">
-        <v>14276.52425</v>
+        <v>-2335.422029999892</v>
       </c>
     </row>
     <row r="118">
@@ -15272,28 +15272,28 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>-1723.561119999863</v>
+        <v>-1332.77090000009</v>
       </c>
       <c r="D134" t="n">
-        <v>-480.5641199998969</v>
+        <v>-289.8369599999446</v>
       </c>
       <c r="E134" t="n">
-        <v>-1005.532439999966</v>
+        <v>-672.3995099998965</v>
       </c>
       <c r="F134" t="n">
-        <v>-680.851949999838</v>
+        <v>-372.6629400000148</v>
       </c>
       <c r="G134" t="n">
-        <v>-680.9777399999808</v>
+        <v>-353.2089999999157</v>
       </c>
       <c r="H134" t="n">
-        <v>-1364.170039999999</v>
+        <v>-832.3401599999128</v>
       </c>
       <c r="I134" t="n">
-        <v>-874.135509999979</v>
+        <v>-432.75971000002</v>
       </c>
       <c r="J134" t="n">
-        <v>-1042.431509999994</v>
+        <v>-608.6542400000075</v>
       </c>
     </row>
     <row r="135">
@@ -16073,7 +16073,7 @@
         <v>482.4293900001067</v>
       </c>
       <c r="E24" t="n">
-        <v>1767358.67267</v>
+        <v>1118.180709999933</v>
       </c>
       <c r="F24" t="n">
         <v>1218.492799999922</v>
@@ -16094,13 +16094,13 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>1221.446669999978</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>4096.54976999991</v>
+        <v>-1818698.67609</v>
       </c>
       <c r="F25" t="n">
-        <v>1506.043480000017</v>
+        <v>-1818595.78447</v>
       </c>
     </row>
     <row r="26">
@@ -16502,13 +16502,13 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>651.5766499999245</v>
+        <v>627.5567000000137</v>
       </c>
       <c r="E42" t="n">
-        <v>836.2998999998581</v>
+        <v>946.9636000001174</v>
       </c>
       <c r="F42" t="n">
-        <v>1034.118519999993</v>
+        <v>936.9099900000037</v>
       </c>
     </row>
     <row r="43">
@@ -17177,7 +17177,7 @@
         <v>603.2153202520078</v>
       </c>
       <c r="E70" t="n">
-        <v>1767331.838991269</v>
+        <v>1091.347031269382</v>
       </c>
       <c r="F70" t="n">
         <v>1466.290272148075</v>
@@ -17198,13 +17198,13 @@
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>1321.900010251881</v>
+        <v>101.5960702519012</v>
       </c>
       <c r="E71" t="n">
-        <v>4119.545781269374</v>
+        <v>-1818675.262898731</v>
       </c>
       <c r="F71" t="n">
-        <v>1795.967132148192</v>
+        <v>-1818304.322037852</v>
       </c>
     </row>
     <row r="72">
@@ -17606,13 +17606,13 @@
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>741.7793102518256</v>
+        <v>687.2184702519155</v>
       </c>
       <c r="E88" t="n">
-        <v>815.1823412693054</v>
+        <v>851.1181012695657</v>
       </c>
       <c r="F88" t="n">
-        <v>1232.373732148146</v>
+        <v>1308.908902148157</v>
       </c>
     </row>
     <row r="89">
@@ -18158,7 +18158,7 @@
         <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>1797371.06345</v>
+        <v>277.2569100000055</v>
       </c>
       <c r="E111" t="n">
         <v>479.0264299999762</v>
@@ -18182,13 +18182,13 @@
         <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>408.8980200001515</v>
+        <v>-456.7116499999884</v>
       </c>
       <c r="E112" t="n">
-        <v>710.7362000001558</v>
+        <v>-811.5589799999725</v>
       </c>
       <c r="F112" t="n">
-        <v>1815.751910000017</v>
+        <v>1718439.20091</v>
       </c>
     </row>
     <row r="113">
@@ -18449,7 +18449,7 @@
         <v>177.822180000021</v>
       </c>
       <c r="E123" t="n">
-        <v>1388758.51766</v>
+        <v>597.7941300000111</v>
       </c>
       <c r="F123" t="n">
         <v>733.4807300001103</v>
@@ -18590,13 +18590,13 @@
         <v>0</v>
       </c>
       <c r="D129" t="n">
-        <v>-25.90611000005083</v>
+        <v>184.2722599999433</v>
       </c>
       <c r="E129" t="n">
-        <v>642.875869999898</v>
+        <v>551.1843599999793</v>
       </c>
       <c r="F129" t="n">
-        <v>486.0012799999822</v>
+        <v>599.9825000001238</v>
       </c>
     </row>
     <row r="130">
@@ -19262,7 +19262,7 @@
         <v>0</v>
       </c>
       <c r="D157" t="n">
-        <v>1797346.163829606</v>
+        <v>252.3572896063319</v>
       </c>
       <c r="E157" t="n">
         <v>552.3406196357482</v>
@@ -19286,13 +19286,13 @@
         <v>0</v>
       </c>
       <c r="D158" t="n">
-        <v>425.3705696064733</v>
+        <v>-440.1626503936649</v>
       </c>
       <c r="E158" t="n">
-        <v>782.6412096359247</v>
+        <v>-739.2851903642013</v>
       </c>
       <c r="F158" t="n">
-        <v>2063.469493892618</v>
+        <v>1718686.363753892</v>
       </c>
     </row>
     <row r="159">
@@ -19553,7 +19553,7 @@
         <v>131.9360496063455</v>
       </c>
       <c r="E169" t="n">
-        <v>1388806.253449636</v>
+        <v>645.5299196357818</v>
       </c>
       <c r="F169" t="n">
         <v>934.0729938927125</v>
@@ -19694,13 +19694,13 @@
         <v>0</v>
       </c>
       <c r="D175" t="n">
-        <v>-55.22651039372556</v>
+        <v>122.3432496062681</v>
       </c>
       <c r="E175" t="n">
-        <v>691.3694696356691</v>
+        <v>639.2674796357502</v>
       </c>
       <c r="F175" t="n">
-        <v>687.3188538925854</v>
+        <v>950.6240338927262</v>
       </c>
     </row>
     <row r="176">
@@ -20246,13 +20246,13 @@
         <v>0</v>
       </c>
       <c r="D198" t="n">
-        <v>1797784.5341</v>
+        <v>-25.54809999992358</v>
       </c>
       <c r="E198" t="n">
         <v>952.1645800000442</v>
       </c>
       <c r="F198" t="n">
-        <v>1797784.5341</v>
+        <v>1495.66219999997</v>
       </c>
     </row>
     <row r="199">
@@ -20270,13 +20270,13 @@
         <v>0</v>
       </c>
       <c r="D199" t="n">
-        <v>-1168.807529999867</v>
+        <v>2145.399510000061</v>
       </c>
       <c r="E199" t="n">
-        <v>-1561.225139999806</v>
+        <v>688.8271000000259</v>
       </c>
       <c r="F199" t="n">
-        <v>1744.887710000057</v>
+        <v>1769.692060000125</v>
       </c>
     </row>
     <row r="200">
@@ -20678,13 +20678,13 @@
         <v>0</v>
       </c>
       <c r="D216" t="n">
-        <v>-98.89343000008921</v>
+        <v>216.5076899998439</v>
       </c>
       <c r="E216" t="n">
-        <v>1111.911109999937</v>
+        <v>989.8829999999634</v>
       </c>
       <c r="F216" t="n">
-        <v>1229.045320000068</v>
+        <v>1377.15161999995</v>
       </c>
     </row>
     <row r="217">
@@ -21350,13 +21350,13 @@
         <v>0</v>
       </c>
       <c r="D244" t="n">
-        <v>1797816.505340345</v>
+        <v>6.423140344577803</v>
       </c>
       <c r="E244" t="n">
         <v>999.1260489045219</v>
       </c>
       <c r="F244" t="n">
-        <v>1797529.651567285</v>
+        <v>1240.779667284732</v>
       </c>
     </row>
     <row r="245">
@@ -21374,13 +21374,13 @@
         <v>0</v>
       </c>
       <c r="D245" t="n">
-        <v>-1089.509899655364</v>
+        <v>2278.418590344562</v>
       </c>
       <c r="E245" t="n">
-        <v>-1493.399171095333</v>
+        <v>760.3308889044948</v>
       </c>
       <c r="F245" t="n">
-        <v>1316.252437284819</v>
+        <v>1368.223187284885</v>
       </c>
     </row>
     <row r="246">
@@ -21782,13 +21782,13 @@
         <v>0</v>
       </c>
       <c r="D262" t="n">
-        <v>-83.07988965558778</v>
+        <v>87.74002034434525</v>
       </c>
       <c r="E262" t="n">
-        <v>1167.153238904408</v>
+        <v>1042.200948904434</v>
       </c>
       <c r="F262" t="n">
-        <v>999.9879772848283</v>
+        <v>1584.79890728471</v>
       </c>
     </row>
   </sheetData>
@@ -22159,13 +22159,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>100000</v>
+        <v>1975.668560000031</v>
       </c>
       <c r="D22" t="n">
-        <v>100000</v>
+        <v>1888.764979999905</v>
       </c>
     </row>
     <row r="23">
@@ -22450,10 +22450,10 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>1208.017700000255</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>1050.027980000323</v>
       </c>
     </row>
   </sheetData>
@@ -23115,10 +23115,10 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>4008.140355459685</v>
+        <v>1954.03404545994</v>
       </c>
       <c r="D40" t="n">
-        <v>4269.678757660915</v>
+        <v>1987.642837661236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalise data for submission
</commit_message>
<xml_diff>
--- a/XLSX/data.xlsx
+++ b/XLSX/data.xlsx
@@ -6804,20 +6804,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="O1:Z1"/>
     <mergeCell ref="AA1:AL1"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="K2:N2"/>
     <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="O1:Z1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="AE2:AH2"/>
     <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -11359,8 +11359,8 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="C1:K1"/>
     <mergeCell ref="L1:T1"/>
-    <mergeCell ref="C1:K1"/>
     <mergeCell ref="U1:AC1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15674,13 +15674,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="C1:O1"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="T2:W2"/>
     <mergeCell ref="P1:AB1"/>
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="X2:AA2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>